<commit_message>
Bai 21 : Excel VSTO
</commit_message>
<xml_diff>
--- a/ExcelWorkbook1/ExcelWorkbook1.xlsx
+++ b/ExcelWorkbook1/ExcelWorkbook1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kysudo\source\repos\BIMSoftVN\K009\ExcelWorkbook1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4EF084-A9D1-44DA-B997-0A1707D742D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C20EB46-5165-4322-ADC0-C52ACD4274E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{BA5D427A-EC69-429B-A005-CF2CD505C356}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{BA5D427A-EC69-429B-A005-CF2CD505C356}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -126,6 +126,895 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Nhiệt độ</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B8E1-49F5-ABEB-74516EE3586E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="290787920"/>
+        <c:axId val="281993536"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="290787920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="281993536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="281993536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="290787920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47631</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123831</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="BieuDo1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AF82406-8C2D-9002-6345-30F10B45BC76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -449,7 +1338,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,5 +1469,6 @@
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>